<commit_message>
Added concurrency to the scraping process
</commit_message>
<xml_diff>
--- a/upgrade.xlsx
+++ b/upgrade.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Wzmacniacz gitarowy - Legnica" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Kolumna gitarowa - Legnica" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Wmzacniacz gitarowy - Zagan" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Wzmacniacz gitarowy - Zagan" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Kolumna gitarowa - Zagan" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Orange gitarowy - Legnica" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Mxr micro amp" sheetId="6" state="visible" r:id="rId6"/>
@@ -517,17 +517,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zoom G3X!! Super Efekt!! Wysylka gratis!!</t>
+          <t>Wzmacniacz lampowy combo Orange Rocker 32</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>450 zł</t>
+          <t>4 500 zł</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Zawidów</t>
+          <t>Wrocław, Fabryczna</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -536,41 +536,41 @@
         </is>
       </c>
       <c r="E3">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/zoom-g3x-super-efekt-wysylka-gratis-CID751-IDYsXVp.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-combo-orange-rocker-32-CID751-IDYsepR.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F3">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/j5l65dal1tg92-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/ld3xr9h8bm0q2-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Wzmacniacz lampowy Fender Champ x2</t>
+          <t>Zoom G3X!! Super Efekt!! Wysylka gratis!!</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1 900 zł</t>
+          <t>450 zł</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Świebodzice</t>
+          <t>Zawidów</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>29 stycznia 2024</t>
         </is>
       </c>
       <c r="E4">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-fender-champ-x2-CID751-IDYm2ZN.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/zoom-g3x-super-efekt-wysylka-gratis-CID751-IDYsXVp.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F4">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/cgbmv9p8ovga-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/j5l65dal1tg92-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
@@ -847,26 +847,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Victory VC35 Copper wzmacniacz lampowy typu Vox Matchless</t>
+          <t>Cornford 212 V30 8 Ohm kolumna gitarowa (jak Marshall, Soldano, Mesa)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4 500 zł</t>
+          <t>3 700 zł</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Wrocław, Stare Miasto</t>
+          <t>Wrocław, Fabryczna</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>07 stycznia 2024</t>
         </is>
       </c>
       <c r="E14">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/victory-vc35-copper-wzmacniacz-lampowy-typu-vox-matchless-CID751-IDVxBOz.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-212-v30-8-ohm-kolumna-gitarowa-jak-marshall-soldano-mesa-CID751-IDYaipP.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F14">
@@ -877,12 +877,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Wzmacniacz lampowy combo Orange Rocker 32</t>
+          <t>Cornford MK50 UK (jak Marshall, Soldano)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4 500 zł</t>
+          <t>9 500 zł</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -892,11 +892,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>29 stycznia 2024</t>
+          <t>28 stycznia 2024</t>
         </is>
       </c>
       <c r="E15">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-combo-orange-rocker-32-CID751-IDYsepR.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-mk50-uk-jak-marshall-soldano-CID751-IDY1Keo.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F15">
@@ -1237,26 +1237,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Marshall JCM 800 model 2210 po pełnym serwisie 1989r.</t>
+          <t>Wzmacniacz lampowy Fender Champ x2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6 800 zł</t>
+          <t>1 900 zł</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Legnica</t>
+          <t>Świebodzice</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>22 stycznia 2024</t>
+          <t>28 stycznia 2024</t>
         </is>
       </c>
       <c r="E27">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm-800-model-2210-po-pelnym-serwisie-1989r-CID751-IDYp5dX.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-fender-champ-x2-CID751-IDYm2ZN.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F27">
@@ -1297,26 +1297,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Cornford MK50 UK (jak Marshall, Soldano)</t>
+          <t>Marshall JCM 800 model 2210 po pełnym serwisie 1989r.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>9 500 zł</t>
+          <t>6 800 zł</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Legnica</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>22 stycznia 2024</t>
         </is>
       </c>
       <c r="E29">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-mk50-uk-jak-marshall-soldano-CID751-IDY1Keo.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm-800-model-2210-po-pelnym-serwisie-1989r-CID751-IDYp5dX.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F29">
@@ -1627,26 +1627,26 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Cornford 212 V30 8 Ohm kolumna gitarowa (jak Marshall, Soldano, Mesa)</t>
+          <t>Victory VC35 Copper wzmacniacz lampowy typu Vox Matchless</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3 700 zł</t>
+          <t>4 500 zł</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Wrocław, Stare Miasto</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>07 stycznia 2024</t>
+          <t>28 stycznia 2024</t>
         </is>
       </c>
       <c r="E40">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-212-v30-8-ohm-kolumna-gitarowa-jak-marshall-soldano-mesa-CID751-IDYaipP.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/victory-vc35-copper-wzmacniacz-lampowy-typu-vox-matchless-CID751-IDVxBOz.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F40">
@@ -3612,7 +3612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3693,30 +3693,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cornford MK50 UK (jak Marshall, Soldano)</t>
+          <t>Marshall JCM 800 model 2210 po pełnym serwisie 1989r.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9 500 zł</t>
+          <t>6 800 zł</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Legnica</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>22 stycznia 2024</t>
         </is>
       </c>
       <c r="E3">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-mk50-uk-jak-marshall-soldano-CID751-IDY1Keo.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm-800-model-2210-po-pelnym-serwisie-1989r-CID751-IDYp5dX.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F3">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/ssz4tp7kq4q11-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/wcvgb2ll7thl3-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
@@ -4053,26 +4053,26 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Marshall JCM 800 model 2210 po pełnym serwisie 1989r.</t>
+          <t>Cornford MK50 UK (jak Marshall, Soldano)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6 800 zł</t>
+          <t>9 500 zł</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Legnica</t>
+          <t>Wrocław, Fabryczna</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>22 stycznia 2024</t>
+          <t>28 stycznia 2024</t>
         </is>
       </c>
       <c r="E15">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm-800-model-2210-po-pelnym-serwisie-1989r-CID751-IDYp5dX.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-mk50-uk-jak-marshall-soldano-CID751-IDY1Keo.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F15">
@@ -4383,17 +4383,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Cornford MK50 UK (jak Marshall, Soldano)</t>
+          <t>Wzmacniacz i kolumny</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>9 500 zł</t>
+          <t>500 zł</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Oława</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -4402,7 +4402,7 @@
         </is>
       </c>
       <c r="E26">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/cornford-mk50-uk-jak-marshall-soldano-CID751-IDY1Keo.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-i-kolumny-CID99-IDT0CeY.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F26">
@@ -4413,17 +4413,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Wzmacniacz i kolumny</t>
+          <t>Kolumna gitarowa Kustom KG412 - 4x12", 120 W RMS,</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>500 zł</t>
+          <t>790 zł</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Oława</t>
+          <t>Zgorzelec</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4432,7 +4432,7 @@
         </is>
       </c>
       <c r="E27">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-i-kolumny-CID99-IDT0CeY.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-kustom-kg412-4x12-120-w-rms-CID751-IDYtHDL.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F27">
@@ -4443,12 +4443,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Kolumna gitarowa Kustom KG412 - 4x12", 120 W RMS,</t>
+          <t>Głowa i kolumna gitarowa Marshall MG100HCFX + Kustom KG412,</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>790 zł</t>
+          <t>1 600 zł</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -4462,7 +4462,7 @@
         </is>
       </c>
       <c r="E28">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-kustom-kg412-4x12-120-w-rms-CID751-IDYtHDL.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/glowa-i-kolumna-gitarowa-marshall-mg100hcfx-kustom-kg412-CID751-IDXuETX.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F28">
@@ -4473,26 +4473,26 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Głowa i kolumna gitarowa Marshall MG100HCFX + Kustom KG412,</t>
+          <t>Wzmacniacz gitarowy Marshall CODE 50C</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1 600 zł</t>
+          <t>900 zł</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Zgorzelec</t>
+          <t>Wrocław, Fabryczna</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>27 stycznia 2024</t>
         </is>
       </c>
       <c r="E29">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/glowa-i-kolumna-gitarowa-marshall-mg100hcfx-kustom-kg412-CID751-IDXuETX.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-marshall-code-50c-CID751-IDYtEya.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F29">
@@ -4503,17 +4503,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Wzmacniacz gitarowy Marshall CODE 50C</t>
+          <t>Kolumna gitarowa Teisco Japonia</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>900 zł</t>
+          <t>599 zł</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Bielawa</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="E30">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-marshall-code-50c-CID751-IDYtEya.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-teisco-japonia-CID751-IDXFo9j.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F30">
@@ -4533,17 +4533,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kolumna gitarowa Teisco Japonia</t>
+          <t>Kruger &amp; Martz Stage One</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>599 zł</t>
+          <t>700 zł</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bielawa</t>
+          <t>Kamienna Góra</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="E31">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-teisco-japonia-CID751-IDXFo9j.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kruger-martz-stage-one-CID99-IDY5IkX.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F31">
@@ -4563,17 +4563,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Kruger &amp; Martz Stage One</t>
+          <t>Kolumna glośnik auna bluetooth usb sd led</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>700 zł</t>
+          <t>650 zł</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Kamienna Góra</t>
+          <t>Wrocław, Krzyki</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -4582,7 +4582,7 @@
         </is>
       </c>
       <c r="E32">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kruger-martz-stage-one-CID99-IDY5IkX.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-glosnik-auna-bluetooth-usb-sd-led-CID99-IDYmXOH.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F32">
@@ -4593,17 +4593,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Wzmacniacz gitarowy Soundman mk4 Full lampa plus  pokrowiec</t>
+          <t>Kolumna gitarowa Buzzaro 212ST-B</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>950 zł</t>
+          <t>1 700 zł</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Krzywiń</t>
+          <t>Jarocin</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="E33">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-soundman-mk4-full-lampa-plus-pokrowiec-CID751-IDYtrlW.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-buzzaro-212st-b-CID751-IDXokrV.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F33">
@@ -4623,17 +4623,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Kolumna glośnik auna bluetooth usb sd led</t>
+          <t>Marshall JCM900 100W Hi Gain Dual Reverb + Kolumna Marshalla + Footsw.</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>650 zł</t>
+          <t>2 999 zł</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Wrocław, Krzyki</t>
+          <t>Bielawa</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="E34">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-glosnik-auna-bluetooth-usb-sd-led-CID99-IDYmXOH.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm900-100w-hi-gain-dual-reverb-kolumna-marshalla-footsw-CID751-IDVTRmy.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F34">
@@ -4653,17 +4653,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Kolumna gitarowa Buzzaro 212ST-B</t>
+          <t>Antelope Audio Orion Studio Synergy Core + GRATIS MIKROFON</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1 700 zł</t>
+          <t>9 999 zł</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Jarocin</t>
+          <t>Kiełczów</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -4672,7 +4672,7 @@
         </is>
       </c>
       <c r="E35">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-buzzaro-212st-b-CID751-IDXokrV.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/antelope-audio-orion-studio-synergy-core-gratis-mikrofon-CID99-IDX63BQ.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F35">
@@ -4683,17 +4683,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Marshall JCM900 100W Hi Gain Dual Reverb + Kolumna Marshalla + Footsw.</t>
+          <t>Music Man HD-130 Reverb plus kolumna 4x12</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2 999 zł</t>
+          <t>8 000 zł</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bielawa</t>
+          <t>Srebrna Góra</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -4702,7 +4702,7 @@
         </is>
       </c>
       <c r="E36">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm900-100w-hi-gain-dual-reverb-kolumna-marshalla-footsw-CID751-IDVTRmy.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/music-man-hd-130-reverb-plus-kolumna-4x12-CID751-IDRUcxW.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F36">
@@ -4713,17 +4713,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Antelope Audio Orion Studio Synergy Core + GRATIS MIKROFON</t>
+          <t>YAMAHA NS-G30 MK II, kolumny, monitory stereo HI-FI. Moc 100 Watt.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>9 999 zł</t>
+          <t>430 zł</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Kiełczów</t>
+          <t>Lubin</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="E37">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/antelope-audio-orion-studio-synergy-core-gratis-mikrofon-CID99-IDX63BQ.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/yamaha-ns-g30-mk-ii-kolumny-monitory-stereo-hi-fi-moc-100-watt-CID99-IDXjO63.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F37">
@@ -4743,26 +4743,26 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Music Man HD-130 Reverb plus kolumna 4x12</t>
+          <t>Wzmacniacz lampowy gitarowy higain Ashdown FallenAngel 60w</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8 000 zł</t>
+          <t>1 550 zł</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Srebrna Góra</t>
+          <t>Jarocin</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>27 stycznia 2024</t>
+          <t>26 stycznia 2024</t>
         </is>
       </c>
       <c r="E38">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/music-man-hd-130-reverb-plus-kolumna-4x12-CID751-IDRUcxW.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-gitarowy-higain-ashdown-fallenangel-60w-CID751-IDYfnbc.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F38">
@@ -4773,26 +4773,26 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>YAMAHA NS-G30 MK II, kolumny, monitory stereo HI-FI. Moc 100 Watt.</t>
+          <t>Kolumna gitarowa Hiwatt M412 + S412 800w</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>430 zł</t>
+          <t>1 500 zł</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lubin</t>
+          <t>Jarocin</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>27 stycznia 2024</t>
+          <t>26 stycznia 2024</t>
         </is>
       </c>
       <c r="E39">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/yamaha-ns-g30-mk-ii-kolumny-monitory-stereo-hi-fi-moc-100-watt-CID99-IDXjO63.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-hiwatt-m412-s412-800w-CID751-IDYfnPW.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F39">
@@ -4803,17 +4803,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Wzmacniacz lampowy gitarowy higain Ashdown FallenAngel 60w</t>
+          <t>Wzmacniacz gitarowy Line 6 DT25 combo</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1 550 zł</t>
+          <t>1 860 zł</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jarocin</t>
+          <t>Kąty Wrocławskie</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -4822,7 +4822,7 @@
         </is>
       </c>
       <c r="E40">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-gitarowy-higain-ashdown-fallenangel-60w-CID751-IDYfnbc.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-line-6-dt25-combo-CID751-IDXAgU1.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F40">
@@ -4833,17 +4833,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Kolumna gitarowa Hiwatt M412 + S412 800w</t>
+          <t>Harley Benton G412S kolumna gitarowa</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1 500 zł</t>
+          <t>650 zł</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Jarocin</t>
+          <t>Lubomierz</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -4852,7 +4852,7 @@
         </is>
       </c>
       <c r="E41">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-hiwatt-m412-s412-800w-CID751-IDYfnPW.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/harley-benton-g412s-kolumna-gitarowa-CID751-IDXvgIl.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F41">
@@ -4863,26 +4863,26 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Wzmacniacz gitarowy Line 6 DT25 combo</t>
+          <t>Kolumna gitarowa  2x12 case glosniki celestion rola</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1 860 zł</t>
+          <t>2 200 zł</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Kąty Wrocławskie</t>
+          <t>Leszno</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>26 stycznia 2024</t>
+          <t>25 stycznia 2024</t>
         </is>
       </c>
       <c r="E42">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-line-6-dt25-combo-CID751-IDXAgU1.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-2x12-case-glosniki-celestion-rola-CID751-IDWqizN.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F42">
@@ -4893,26 +4893,26 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Harley Benton G412S kolumna gitarowa</t>
+          <t>BUDDA 4x12 Closed Back Cab kolumna gitarowa</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>650 zł</t>
+          <t>3 500 zł</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Lubomierz</t>
+          <t>Dzierżoniów</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>26 stycznia 2024</t>
+          <t>25 stycznia 2024</t>
         </is>
       </c>
       <c r="E43">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/harley-benton-g412s-kolumna-gitarowa-CID751-IDXvgIl.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/budda-4x12-closed-back-cab-kolumna-gitarowa-CID751-IDYrJXE.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F43">
@@ -4923,17 +4923,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Kolumna gitarowa  2x12 case glosniki celestion rola</t>
+          <t>Wieża stereo Głośnik LG XBOOM RN5</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2 200 zł</t>
+          <t>799 zł</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Leszno</t>
+          <t>Bolesławiec</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="E44">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-2x12-case-glosniki-celestion-rola-CID751-IDWqizN.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wieza-stereo-glosnik-lg-xboom-rn5-CID99-IDYrsMO.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F44">
@@ -4953,17 +4953,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>BUDDA 4x12 Closed Back Cab kolumna gitarowa</t>
+          <t>Kustom 100KG FX112</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3 500 zł</t>
+          <t>499 zł</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Dzierżoniów</t>
+          <t>Milicz</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4972,40 +4972,10 @@
         </is>
       </c>
       <c r="E45">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/budda-4x12-closed-back-cab-kolumna-gitarowa-CID751-IDYrJXE.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kustom-100kg-fx112-CID99-IDYrpf3.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F45">
-        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Wieża stereo Głośnik LG XBOOM RN5</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>799 zł</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Bolesławiec</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>25 stycznia 2024</t>
-        </is>
-      </c>
-      <c r="E46">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wieza-stereo-glosnik-lg-xboom-rn5-CID99-IDYrsMO.html", "item_url, click to access")</f>
-        <v/>
-      </c>
-      <c r="F46">
         <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
         <v/>
       </c>
@@ -5021,14 +4991,1375 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="68" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>item_url</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>photo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Fender Blues Junior IV</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2 100 zł</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Głogów</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E2">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/fender-blues-junior-iv-CID751-IDYmEXj.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/xnmb1mms1zvn1-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Marshall JCM 800 model 2210 po pełnym serwisie 1989r.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6 800 zł</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Legnica</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>22 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E3">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jcm-800-model-2210-po-pelnym-serwisie-1989r-CID751-IDYp5dX.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F3">
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/wcvgb2ll7thl3-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Zoom G3X!! Super Efekt!! Wysylka gratis!!</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>450 zł</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Zawidów</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E4">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/zoom-g3x-super-efekt-wysylka-gratis-CID751-IDYsXVp.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/j5l65dal1tg92-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Koch The Grek Koch</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10 000 zł</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Złotoryja</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E5">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/koch-the-grek-koch-CID751-IDYahgw.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/8j0el7gkn3703-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy Fender Acoustasonic Junior</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>800 zł</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Legnica</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E6">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-fender-acoustasonic-junior-CID751-IDW9hEj.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F6">
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/97oifcoula2f-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Piec lampowy gitarowy Blackstar</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1 800 zł</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lwówek Śląski</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E7">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/piec-lampowy-gitarowy-blackstar-CID751-IDXndt3.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F7">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Amerykański wzmacniacz do gitary Peavey Pro Studio</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>700 zł</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E8">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/amerykanski-wzmacniacz-do-gitary-peavey-pro-studio-CID751-IDNcsy2.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Amerykański wzmacniacz Peavey na baterie, akumulator 12V</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>400 zł</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E9">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/amerykanski-wzmacniacz-peavey-na-baterie-akumulator-12v-CID751-IDHQJd5.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Blackstar HT-5RS gitarowy wzmacniacz lampowy mini stack,</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1 690 zł</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Głogów</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E10">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/blackstar-ht-5rs-gitarowy-wzmacniacz-lampowy-mini-stack-CID751-IDXc2CB.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Marshall valvestate 2000 avt 150W.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1 600 zł</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Milików</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E11">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-valvestate-2000-avt-150w-CID751-IDY3s1i.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F11">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Piec gitarowy SANO model 500rc Lampowy „vintage” lata 70 USA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2 999 zł</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Głogów</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>30 styczeń 2024</t>
+        </is>
+      </c>
+      <c r="E12">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/piec-gitarowy-sano-model-500rc-lampowy-vintage-lata-70-usa-CID751-IDYwNJy.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F12">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wzmacniacz Hugnes &amp; Kettner Triamp MKII  Head 100 W/50W</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5 900 zł</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Legnica</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E13">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-hugnes-kettner-triamp-mkii-head-100-w-50w-CID751-IDVDxSN.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F13">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Marshall JVM215C Combo wzmacniacz lampowy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>3 399 zł</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Środa Śląska</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E14">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-jvm215c-combo-wzmacniacz-lampowy-CID751-IDX8JLU.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F14">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Wzmacniacz lampowy Fender Champ x2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1 900 zł</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Świebodzice</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E15">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-fender-champ-x2-CID751-IDYm2ZN.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F15">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kolumna - wzmacniacz gitarowy Tonsil</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>380 zł</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Rydzyna</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E16">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-wzmacniacz-gitarowy-tonsil-CID99-IDYwswi.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F16">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy 25w</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>650 zł</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Polkowice Dolne</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E17">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-25w-CID99-IDWg6Ob.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F17">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>One Control Crocodile Tail Loop sterownik gitarowy, looper MIDI</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2 000 zł</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kościan</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E18">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/one-control-crocodile-tail-loop-sterownik-gitarowy-looper-midi-CID99-IDDV8JL.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F18">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy: Fender Mustang III V2</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>950 zł</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Jelenia Góra, Centrum</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E19">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-fender-mustang-iii-v2-CID751-IDVD4mj.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F19">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Zoom G3X!! Super Efekt!! Wysylka gratis!!</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>450 zł</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Zawidów</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E20">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/zoom-g3x-super-efekt-wysylka-gratis-CID751-IDYsXVp.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F20">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wzmacniacz do gitary Hohner</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>350 zł</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E21">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-do-gitary-hohner-CID751-IDXZ5pX.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F21">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Piec gitarowy + Mikrofon Ken Rose, petla efektów, Reverb itd.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>400 zł</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E22">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/piec-gitarowy-mikrofon-ken-rose-petla-efektow-reverb-itd-CID751-IDBzWlk.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F22">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Japoński wzmacniacz do gitary Luxor Solid State Tremolo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>750 zł</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E23">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/japonski-wzmacniacz-do-gitary-luxor-solid-state-tremolo-CID751-IDwiYu3.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F23">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Lampowy wzmacniacz do gitary elektrycznej Drive CD-200RT</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>550 zł</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E24">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/lampowy-wzmacniacz-do-gitary-elektrycznej-drive-cd-200rt-CID751-IDPoDtp.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F24">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Trace Elliot GP7SM - Tranzystorowy Wzmacniacz do gitary basowej</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>800 zł</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Wołów</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>29 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E25">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/trace-elliot-gp7sm-tranzystorowy-wzmacniacz-do-gitary-basowej-CID751-IDXJWHP.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F25">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Multiefekt gitarowy Zoom G11 podłogowy</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2 400 zł</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Karpacz</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E26">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/multiefekt-gitarowy-zoom-g11-podlogowy-CID751-IDTClFJ.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F26">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Kolumna 212 Marshall 1936 / G12T75 -kółka, pokrowiec</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1 500 zł</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Włoszakowice</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E27">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-212-marshall-1936-g12t75-kolka-pokrowiec-CID751-IDYbldx.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F27">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Roland Cube Street EX</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1 850 zł</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Słubice</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E28">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-cube-street-ex-CID99-IDYujZA.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F28">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Boss Katana MK II 100W</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1 400 zł</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Wałbrzych</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E29">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-katana-mk-ii-100w-CID751-IDY4dw8.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F29">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Wzmacniacz lampowy Fender Champ x2</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1 900 zł</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Świebodzice</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E30">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-lampowy-fender-champ-x2-CID751-IDYm2ZN.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F30">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Wzmacniacz Gitarowy Combo 40w Vox Vt40x</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>900 zł</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Jelenia Góra, Centrum</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E31">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-combo-40w-vox-vt40x-CID751-IDY3wfE.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F31">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Orange Rockerverb MKII 50, kolumna Orange 2x12</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>6 999 zł</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Ruszowice</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E32">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/orange-rockerverb-mkii-50-kolumna-orange-2x12-CID751-IDXJ8lO.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F32">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Amerykański wzmacniacz gitarowy Peavey</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>400 zł</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Jędrzychów</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E33">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/amerykanski-wzmacniacz-gitarowy-peavey-CID751-IDIr0wQ.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F33">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy lampowy BLACKSTAR z kolumną</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2 800 zł</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Żagań</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E34">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-lampowy-blackstar-z-kolumna-CID751-IDXdELf.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F34">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy Peavey RAGE 158 piecyk 15W Blue Marvel</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>320 zł</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Nowy Kisielin</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E35">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-peavey-rage-158-piecyk-15w-blue-marvel-CID99-IDUUHJx.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F35">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Kolumna gitarowa Hughes&amp;Kettner TM212 (2xV30)</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1 400 zł</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Legnickie Pole</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E36">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-hughes-kettner-tm212-2xv30-CID751-IDVRmpY.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F36">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Fender Champion 40</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>550 zł</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Wałbrzych</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E37">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/fender-champion-40-CID751-IDYcPMH.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F37">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Kolumna gitarowa Kustom KG412 - 4x12", 120 W RMS,</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>790 zł</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Zgorzelec</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E38">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kolumna-gitarowa-kustom-kg412-4x12-120-w-rms-CID751-IDYtHDL.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F38">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy Marshall MG100HCFX (głowa gitarowa) z footswitch</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>950 zł</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Zgorzelec</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E39">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-marshall-mg100hcfx-glowa-gitarowa-z-footswitch-CID751-IDYtHya.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F39">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Głowa i kolumna gitarowa Marshall MG100HCFX + Kustom KG412,</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1 600 zł</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Zgorzelec</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>28 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E40">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/glowa-i-kolumna-gitarowa-marshall-mg100hcfx-kustom-kg412-CID751-IDXuETX.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F40">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy Fender Mustang III (V2)</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>700 zł</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Kościan</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>27 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E41">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-fender-mustang-iii-v2-CID751-IDYfGHr.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F41">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy piecyk Vox</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>550 zł</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Sulechów</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>27 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E42">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-piecyk-vox-CID751-IDX6GEl.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F42">
+        <f>HYPERLINK("None", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Wzmacniacz fender rumblr 25</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>520 zł</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wilków</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>27 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E43">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-fender-rumblr-25-CID751-IDYt5rQ.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F43">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Wzmacniacz gitarowy 30w</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>200 zł</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Przemków</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>27 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E44">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-30w-CID751-IDYbUcQ.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F44">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Roland CUBE 20XL wzmacniacz gitarowy z procesorem efektów jak nowy</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>499 zł</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Nowa Sól</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>27 stycznia 2024</t>
+        </is>
+      </c>
+      <c r="E45">
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-cube-20xl-wzmacniacz-gitarowy-z-procesorem-efektow-jak-nowy-CID751-IDVATZC.html", "item_url, click to access")</f>
+        <v/>
+      </c>
+      <c r="F45">
+        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6956,7 +8287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7007,47 +8338,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Boss CE 3 Chorus efekt gitarowy Vintage</t>
+          <t>Boss Chorus Ensemble CE-5 efekt gitarowy Chorus</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>540 zł</t>
+          <t>500 zł</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Płock</t>
+          <t>Zabrze</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24 stycznia 2024</t>
+          <t>30 styczeń 2024</t>
         </is>
       </c>
       <c r="E2">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorus-efekt-gitarowy-vintage-CID751-IDYq4Si.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-efekt-gitarowy-chorus-CID751-IDYjo9x.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F2">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/ajpa8nj86cak3-PL/image;r=90;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/2a7em1pmzd1r-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Boss Ce-3 Chorusa Made in Japan + gratis</t>
+          <t>Maxon ASC10 Ambient Stereo Chorus analogowy efekt gitarowy</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>550 zł</t>
+          <t>639 zł</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Żary</t>
+          <t>Subkowy</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7056,28 +8387,28 @@
         </is>
       </c>
       <c r="E3">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorusa-made-in-japan-gratis-CID751-IDYvrCq.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/maxon-asc10-ambient-stereo-chorus-analogowy-efekt-gitarowy-CID751-IDXops3.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F3">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/lyii53oyd86j1-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/6agdksjkbhxa3-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Boss Super Chorus CH-1</t>
+          <t>Boss Ce-3 Chorusa Made in Japan + gratis</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>255 zł</t>
+          <t>550 zł</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mosina</t>
+          <t>Żary</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -7086,28 +8417,28 @@
         </is>
       </c>
       <c r="E4">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-super-chorus-ch-1-CID751-IDYv7RW.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorusa-made-in-japan-gratis-CID751-IDYvrCq.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F4">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/qbtg5vptecqe2-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/lyii53oyd86j1-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Roland RD-2000 | kup NOWY wymień STARY</t>
+          <t>Boss Super Chorus CH-1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10 500 zł</t>
+          <t>255 zł</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ksawerów</t>
+          <t>Mosina</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -7116,58 +8447,58 @@
         </is>
       </c>
       <c r="E5">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-rd-2000-kup-nowy-wymien-stary-CID751-IDFZ3j0.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-super-chorus-ch-1-CID751-IDYv7RW.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F5">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/mslfuhv73jhm1-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/qbtg5vptecqe2-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Boss CE-3 Chorus Made im Japan</t>
+          <t>Roland RD-2000 | kup NOWY wymień STARY</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>650 zł</t>
+          <t>10 500 zł</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bielsko-Biała</t>
+          <t>Ksawerów</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>29 stycznia 2024</t>
+          <t>30 styczeń 2024</t>
         </is>
       </c>
       <c r="E6">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorus-made-im-japan-CID751-IDY4HUg.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-rd-2000-kup-nowy-wymien-stary-CID751-IDFZ3j0.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F6">
-        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/m4i4hh5slxe3-PL/image;s=200x0;q=50", "photo, click to access")</f>
+        <f>HYPERLINK("https://ireland.apollo.olxcdn.com:443/v1/files/mslfuhv73jhm1-PL/image;s=200x0;q=50", "photo, click to access")</f>
         <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cakewalk v-studio 20, Interfejs audio, kontroler DAW</t>
+          <t>Boss CE-3 Chorus Made im Japan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>550 zł</t>
+          <t>650 zł</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Poznań, Jeżyce</t>
+          <t>Bielsko-Biała</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -7176,7 +8507,7 @@
         </is>
       </c>
       <c r="E7">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/cakewalk-v-studio-20-interfejs-audio-kontroler-daw-CID99-IDXE10n.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorus-made-im-japan-CID751-IDY4HUg.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F7">
@@ -7187,17 +8518,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pedały efektów gitarowych</t>
+          <t>Cakewalk v-studio 20, Interfejs audio, kontroler DAW</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1 200 zł</t>
+          <t>550 zł</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wrocław, Fabryczna</t>
+          <t>Poznań, Jeżyce</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -7206,7 +8537,7 @@
         </is>
       </c>
       <c r="E8">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedaly-efektow-gitarowych-CID751-IDWz4Fj.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/cakewalk-v-studio-20-interfejs-audio-kontroler-daw-CID99-IDXE10n.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F8">
@@ -7217,17 +8548,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Boss CH-1 Super chorus</t>
+          <t>Pedały efektów gitarowych</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>350 zł</t>
+          <t>1 200 zł</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Władysławów</t>
+          <t>Wrocław, Fabryczna</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -7236,7 +8567,7 @@
         </is>
       </c>
       <c r="E9">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ch-1-super-chorus-CID751-IDY34bD.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedaly-efektow-gitarowych-CID751-IDWz4Fj.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F9">
@@ -7247,17 +8578,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Boss Super Chorus</t>
+          <t>Boss CH-1 Super chorus</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>260 zł</t>
+          <t>350 zł</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Górki</t>
+          <t>Władysławów</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -7266,7 +8597,7 @@
         </is>
       </c>
       <c r="E10">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-super-chorus-CID751-IDYw0UT.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ch-1-super-chorus-CID751-IDY34bD.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F10">
@@ -7277,17 +8608,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Efekt gitarowy Boss Super Chorus CH-1</t>
+          <t>Boss Super Chorus</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>400 zł</t>
+          <t>260 zł</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Kielce</t>
+          <t>Górki</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -7296,7 +8627,7 @@
         </is>
       </c>
       <c r="E11">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/efekt-gitarowy-boss-super-chorus-ch-1-CID751-IDY496w.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-super-chorus-CID751-IDYw0UT.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F11">
@@ -7307,17 +8638,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Wzmacniacz Roland Jazz-Chorus JC-120 Fabrycznie nowy na gwarancji</t>
+          <t>Efekt gitarowy Boss Super Chorus CH-1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5 800 zł</t>
+          <t>400 zł</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Brzeg Dolny</t>
+          <t>Kielce</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -7326,7 +8657,7 @@
         </is>
       </c>
       <c r="E12">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-roland-jazz-chorus-jc-120-fabrycznie-nowy-na-gwarancji-CID751-IDVBrBc.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/efekt-gitarowy-boss-super-chorus-ch-1-CID751-IDY496w.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F12">
@@ -7337,26 +8668,26 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Joyo DC15 wzmacniacz gitarowy DC-15 combo gitarowe</t>
+          <t>Wzmacniacz Roland Jazz-Chorus JC-120 Fabrycznie nowy na gwarancji</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>399 zł</t>
+          <t>5 800 zł</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Aleksandria Pierwsza</t>
+          <t>Brzeg Dolny</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>28 stycznia 2024</t>
+          <t>29 stycznia 2024</t>
         </is>
       </c>
       <c r="E13">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/joyo-dc15-wzmacniacz-gitarowy-dc-15-combo-gitarowe-CID751-IDXRE5F.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-roland-jazz-chorus-jc-120-fabrycznie-nowy-na-gwarancji-CID751-IDVBrBc.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F13">
@@ -7367,26 +8698,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Grobert The One Chorus (replika Boss CE-1)</t>
+          <t>Joyo DC15 wzmacniacz gitarowy DC-15 combo gitarowe</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>800 zł</t>
+          <t>399 zł</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ostrołęka</t>
+          <t>Aleksandria Pierwsza</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>27 stycznia 2024</t>
+          <t>28 stycznia 2024</t>
         </is>
       </c>
       <c r="E14">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/grobert-the-one-chorus-replika-boss-ce-1-CID751-IDYtBk1.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/joyo-dc15-wzmacniacz-gitarowy-dc-15-combo-gitarowe-CID751-IDXRE5F.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F14">
@@ -7397,17 +8728,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Boss CE-5 Chorus Ensemble - Pink Label - Analog</t>
+          <t>Grobert The One Chorus (replika Boss CE-1)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>750 zł</t>
+          <t>800 zł</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Skawina</t>
+          <t>Ostrołęka</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -7416,7 +8747,7 @@
         </is>
       </c>
       <c r="E15">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-5-chorus-ensemble-pink-label-analog-CID751-IDY1oms.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/grobert-the-one-chorus-replika-boss-ce-1-CID751-IDYtBk1.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F15">
@@ -7427,17 +8758,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Boss chorus CE-5</t>
+          <t>Boss CE-5 Chorus Ensemble - Pink Label - Analog</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>350 zł</t>
+          <t>750 zł</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Kędzierzyn-Koźle, Kłodnica</t>
+          <t>Skawina</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -7446,7 +8777,7 @@
         </is>
       </c>
       <c r="E16">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ce-5-CID751-IDYttBa.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-5-chorus-ensemble-pink-label-analog-CID751-IDY1oms.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F16">
@@ -7457,17 +8788,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Nux MOD Core Deluxe MKII - multiefekt gitarowy</t>
+          <t>Boss chorus CE-5</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>449 zł</t>
+          <t>350 zł</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Puławy</t>
+          <t>Kędzierzyn-Koźle, Kłodnica</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -7476,7 +8807,7 @@
         </is>
       </c>
       <c r="E17">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/nux-mod-core-deluxe-mkii-multiefekt-gitarowy-CID751-IDXfGqD.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ce-5-CID751-IDYttBa.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F17">
@@ -7487,17 +8818,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Super Wzmacniacz Roland Cube Lite Red -efekty-przestery-Boss- wysyłka</t>
+          <t>Nux MOD Core Deluxe MKII - multiefekt gitarowy</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>625 zł</t>
+          <t>449 zł</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bydgoszcz</t>
+          <t>Puławy</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -7506,7 +8837,7 @@
         </is>
       </c>
       <c r="E18">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/super-wzmacniacz-roland-cube-lite-red-efekty-przestery-boss-wysylka-CID751-IDPaEEb.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/nux-mod-core-deluxe-mkii-multiefekt-gitarowy-CID751-IDXfGqD.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F18">
@@ -7517,26 +8848,26 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Boss RC-202 Looper</t>
+          <t>Super Wzmacniacz Roland Cube Lite Red -efekty-przestery-Boss- wysyłka</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1 200 zł</t>
+          <t>625 zł</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Poznań, Łazarz</t>
+          <t>Bydgoszcz</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>26 stycznia 2024</t>
+          <t>27 stycznia 2024</t>
         </is>
       </c>
       <c r="E19">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-rc-202-looper-CID751-IDXxXjG.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/super-wzmacniacz-roland-cube-lite-red-efekty-przestery-boss-wysylka-CID751-IDPaEEb.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F19">
@@ -7547,17 +8878,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>pedalboard ( m.in. boss ce-2 , cioks , lehle ) z combo koch  komplet</t>
+          <t>Boss RC-202 Looper</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11 500 zł</t>
+          <t>1 200 zł</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Płońsk</t>
+          <t>Poznań, Łazarz</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -7566,7 +8897,7 @@
         </is>
       </c>
       <c r="E20">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedalboard-m-in-boss-ce-2-cioks-lehle-z-combo-koch-komplet-CID751-IDY0bQj.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-rc-202-looper-CID751-IDXxXjG.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F20">
@@ -7577,17 +8908,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Boss GT-100 wersja 2.0 multiefekt gitarowy + torba</t>
+          <t>pedalboard ( m.in. boss ce-2 , cioks , lehle ) z combo koch  komplet</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>999 zł</t>
+          <t>11 500 zł</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Piła</t>
+          <t>Płońsk</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -7596,7 +8927,7 @@
         </is>
       </c>
       <c r="E21">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-gt-100-wersja-2-0-multiefekt-gitarowy-torba-CID751-IDXYH4b.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedalboard-m-in-boss-ce-2-cioks-lehle-z-combo-koch-komplet-CID751-IDY0bQj.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F21">
@@ -7607,26 +8938,26 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Wzmacniacz gitarowy combo Line 6 Spider IV 75 W</t>
+          <t>Boss GT-100 wersja 2.0 multiefekt gitarowy + torba</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>600 zł</t>
+          <t>999 zł</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bojano</t>
+          <t>Piła</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>25 stycznia 2024</t>
+          <t>26 stycznia 2024</t>
         </is>
       </c>
       <c r="E22">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-combo-line-6-spider-iv-75-w-CID751-IDYrLjE.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-gt-100-wersja-2-0-multiefekt-gitarowy-torba-CID751-IDXYH4b.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F22">
@@ -7637,17 +8968,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Marshall bass 100 wzmacniacz 2099 vintage lata 70</t>
+          <t>Wzmacniacz gitarowy combo Line 6 Spider IV 75 W</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>899 zł</t>
+          <t>600 zł</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sielpia Wielka</t>
+          <t>Bojano</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -7656,7 +8987,7 @@
         </is>
       </c>
       <c r="E23">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-bass-100-wzmacniacz-2099-vintage-lata-70-CID751-IDUsT8A.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-combo-line-6-spider-iv-75-w-CID751-IDYrLjE.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F23">
@@ -7667,17 +8998,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Boss VE-8 Acoustic Singer</t>
+          <t>Marshall bass 100 wzmacniacz 2099 vintage lata 70</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1 299 zł</t>
+          <t>899 zł</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dębica</t>
+          <t>Sielpia Wielka</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -7686,7 +9017,7 @@
         </is>
       </c>
       <c r="E24">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ve-8-acoustic-singer-CID751-IDWXuZh.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/marshall-bass-100-wzmacniacz-2099-vintage-lata-70-CID751-IDUsT8A.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F24">
@@ -7697,17 +9028,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Boss Chous Ensemble CE-5</t>
+          <t>Boss VE-8 Acoustic Singer</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>330 zł</t>
+          <t>1 299 zł</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Grodzisk Mazowiecki</t>
+          <t>Dębica</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -7716,7 +9047,7 @@
         </is>
       </c>
       <c r="E25">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chous-ensemble-ce-5-CID751-IDYrkjH.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ve-8-acoustic-singer-CID751-IDWXuZh.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F25">
@@ -7727,17 +9058,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Super Wzmacniacz Roland Cube 60-efekty Boss-wyjście na kolumnę-wysyłka</t>
+          <t>Boss Chous Ensemble CE-5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1 050 zł</t>
+          <t>330 zł</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bydgoszcz</t>
+          <t>Grodzisk Mazowiecki</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -7746,7 +9077,7 @@
         </is>
       </c>
       <c r="E26">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/super-wzmacniacz-roland-cube-60-efekty-boss-wyjscie-na-kolumne-wysylka-CID751-IDONqTB.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chous-ensemble-ce-5-CID751-IDYrkjH.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F26">
@@ -7757,26 +9088,26 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Eleven Rack od AVID Procesor Efektów Gitara Bas Wokal</t>
+          <t>Super Wzmacniacz Roland Cube 60-efekty Boss-wyjście na kolumnę-wysyłka</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1 800 zł</t>
+          <t>1 050 zł</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Kraków, Bronowice</t>
+          <t>Bydgoszcz</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>24 stycznia 2024</t>
+          <t>25 stycznia 2024</t>
         </is>
       </c>
       <c r="E27">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/eleven-rack-od-avid-procesor-efektow-gitara-bas-wokal-CID99-IDS0IbU.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/super-wzmacniacz-roland-cube-60-efekty-boss-wyjscie-na-kolumne-wysylka-CID751-IDONqTB.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F27">
@@ -7787,17 +9118,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Roland wzmacniacz do gitary akustycznej</t>
+          <t>Eleven Rack od AVID Procesor Efektów Gitara Bas Wokal</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1 500 zł</t>
+          <t>1 800 zł</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Warszawa, Bielany</t>
+          <t>Kraków, Bronowice</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -7806,7 +9137,7 @@
         </is>
       </c>
       <c r="E28">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-wzmacniacz-do-gitary-akustycznej-CID99-IDXGqZz.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/eleven-rack-od-avid-procesor-efektow-gitara-bas-wokal-CID99-IDS0IbU.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F28">
@@ -7817,17 +9148,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Boss Chorus Ensemble CE-5</t>
+          <t>Roland wzmacniacz do gitary akustycznej</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>300 zł</t>
+          <t>1 500 zł</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Poznań, Jeżyce</t>
+          <t>Warszawa, Bielany</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -7836,7 +9167,7 @@
         </is>
       </c>
       <c r="E29">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-CID751-IDYq7Ww.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/roland-wzmacniacz-do-gitary-akustycznej-CID99-IDXGqZz.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F29">
@@ -7847,17 +9178,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Boss CE 3 Chorus efekt gitarowy Vintage</t>
+          <t>Boss Chorus Ensemble CE-5</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>540 zł</t>
+          <t>300 zł</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Płock</t>
+          <t>Poznań, Jeżyce</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -7866,7 +9197,7 @@
         </is>
       </c>
       <c r="E30">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorus-efekt-gitarowy-vintage-CID751-IDYq4Si.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-CID751-IDYq7Ww.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F30">
@@ -7877,26 +9208,26 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Boss Chorus Ensemble CE-5 efekt gitarowy Chorus</t>
+          <t>Boss CE 3 Chorus efekt gitarowy Vintage</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>500 zł</t>
+          <t>540 zł</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Zabrze</t>
+          <t>Płock</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>23 stycznia 2024</t>
+          <t>24 stycznia 2024</t>
         </is>
       </c>
       <c r="E31">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-efekt-gitarowy-chorus-CID751-IDYjo9x.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-3-chorus-efekt-gitarowy-vintage-CID751-IDYq4Si.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F31">
@@ -7907,17 +9238,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Maxon ASC10 Ambient Stereo Chorus analogowy efekt gitarowy</t>
+          <t>Wzmacniacz gitarowy Roland CUBE 20 X</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>639 zł</t>
+          <t>490 zł</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Subkowy</t>
+          <t>Warszawa, Praga-Południe</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -7926,7 +9257,7 @@
         </is>
       </c>
       <c r="E32">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/maxon-asc10-ambient-stereo-chorus-analogowy-efekt-gitarowy-CID751-IDXops3.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-roland-cube-20-x-CID751-IDYpHHc.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F32">
@@ -7937,17 +9268,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Wzmacniacz gitarowy Roland CUBE 20 X</t>
+          <t>Gwarancja. NUX NAP-5 Stageman Floor - preamp akustyczny z looperem</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>490 zł</t>
+          <t>570 zł</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Warszawa, Praga-Południe</t>
+          <t>Warszawa, Mokotów</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -7956,7 +9287,7 @@
         </is>
       </c>
       <c r="E33">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/wzmacniacz-gitarowy-roland-cube-20-x-CID751-IDYpHHc.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/gwarancja-nux-nap-5-stageman-floor-preamp-akustyczny-z-looperem-CID751-IDUbu0A.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F33">
@@ -7967,26 +9298,26 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Gwarancja. NUX NAP-5 Stageman Floor - preamp akustyczny z looperem</t>
+          <t>BOSS GT-6 Multiefekt Gitarowy</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>570 zł</t>
+          <t>600 zł</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Warszawa, Mokotów</t>
+          <t>Białystok, Centrum</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>23 stycznia 2024</t>
+          <t>22 stycznia 2024</t>
         </is>
       </c>
       <c r="E34">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/gwarancja-nux-nap-5-stageman-floor-preamp-akustyczny-z-looperem-CID751-IDUbu0A.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-gt-6-multiefekt-gitarowy-CID99-IDSXhhA.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F34">
@@ -7997,17 +9328,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BOSS GT-6 Multiefekt Gitarowy</t>
+          <t>Multiefekt gitarowy ZOOM G2.1 Nu(Boss,Roland,Korg) chorus,reverb,delay</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>600 zł</t>
+          <t>400 zł</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Białystok, Centrum</t>
+          <t>Rajbrot</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -8016,7 +9347,7 @@
         </is>
       </c>
       <c r="E35">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-gt-6-multiefekt-gitarowy-CID99-IDSXhhA.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/multiefekt-gitarowy-zoom-g2-1-nuboss-roland-korg-chorus-reverb-delay-CID751-IDY7ywF.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F35">
@@ -8027,17 +9358,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Multiefekt gitarowy ZOOM G2.1 Nu(Boss,Roland,Korg) chorus,reverb,delay</t>
+          <t>Boss CE-2B Chorus Japan Gitara / Bass (CE-2) Lata 80te</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>400 zł</t>
+          <t>700 zł</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Rajbrot</t>
+          <t>Gdańsk, Wrzeszcz</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -8046,7 +9377,7 @@
         </is>
       </c>
       <c r="E36">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/multiefekt-gitarowy-zoom-g2-1-nuboss-roland-korg-chorus-reverb-delay-CID751-IDY7ywF.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-2b-chorus-japan-gitara-bass-ce-2-lata-80te-CID751-IDWiYdC.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F36">
@@ -8057,17 +9388,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Boss CE-2B Chorus Japan Gitara / Bass (CE-2) Lata 80te</t>
+          <t>ZESTAW gitara yamaha pacifica, multiefekt, wzmacniacz</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>700 zł</t>
+          <t>1 400 zł</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Gdańsk, Wrzeszcz</t>
+          <t>Sokółka</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -8076,7 +9407,7 @@
         </is>
       </c>
       <c r="E37">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-ce-2b-chorus-japan-gitara-bass-ce-2-lata-80te-CID751-IDWiYdC.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/zestaw-gitara-yamaha-pacifica-multiefekt-wzmacniacz-CID751-IDXXCXp.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F37">
@@ -8087,17 +9418,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ZESTAW gitara yamaha pacifica, multiefekt, wzmacniacz</t>
+          <t>Kurtka Przejściowa Hugo Boss model Chorus nowa XL</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1 400 zł</t>
+          <t>650 zł</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sokółka</t>
+          <t>Łódź, Górna</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -8106,7 +9437,7 @@
         </is>
       </c>
       <c r="E38">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/zestaw-gitara-yamaha-pacifica-multiefekt-wzmacniacz-CID751-IDXXCXp.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/kurtka-przejsciowa-hugo-boss-model-chorus-nowa-xl-CID87-IDRIVoi.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F38">
@@ -8117,26 +9448,26 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Kurtka Przejściowa Hugo Boss model Chorus nowa XL</t>
+          <t>Combo basowe Boss Dual Cube Bass LX</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>650 zł</t>
+          <t>1 100 zł</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Łódź, Górna</t>
+          <t>Siekierki Wielkie</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>22 stycznia 2024</t>
+          <t>21 stycznia 2024</t>
         </is>
       </c>
       <c r="E39">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/kurtka-przejsciowa-hugo-boss-model-chorus-nowa-xl-CID87-IDRIVoi.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/combo-basowe-boss-dual-cube-bass-lx-CID751-IDXEGGe.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F39">
@@ -8147,17 +9478,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Combo basowe Boss Dual Cube Bass LX</t>
+          <t>Boss Chorus Ensemble CE-5</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1 100 zł</t>
+          <t>350 zł</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Siekierki Wielkie</t>
+          <t>Poznań, Jeżyce</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -8166,7 +9497,7 @@
         </is>
       </c>
       <c r="E40">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/combo-basowe-boss-dual-cube-bass-lx-CID751-IDXEGGe.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-CID751-IDYnyp6.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F40">
@@ -8177,17 +9508,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Boss Chorus Ensemble CE-5</t>
+          <t>Pedalboard z efektami</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>350 zł</t>
+          <t>1 200 zł</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Poznań, Jeżyce</t>
+          <t>Pszczyna</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -8196,40 +9527,10 @@
         </is>
       </c>
       <c r="E41">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/boss-chorus-ensemble-ce-5-CID751-IDYnyp6.html", "item_url, click to access")</f>
+        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedalboard-z-efektami-CID751-IDYaUL8.html", "item_url, click to access")</f>
         <v/>
       </c>
       <c r="F41">
-        <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Pedalboard z efektami</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>1 200 zł</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Pszczyna</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>21 stycznia 2024</t>
-        </is>
-      </c>
-      <c r="E42">
-        <f>HYPERLINK("https://www.olx.pl/d/oferta/pedalboard-z-efektami-CID751-IDYaUL8.html", "item_url, click to access")</f>
-        <v/>
-      </c>
-      <c r="F42">
         <f>HYPERLINK("/app/static/media/no_thumbnail.15f456ec5.svg", "photo, click to access")</f>
         <v/>
       </c>

</xml_diff>